<commit_message>
updated information in risk management and time estimation
</commit_message>
<xml_diff>
--- a/docs/sem_2/risk_management.xlsx
+++ b/docs/sem_2/risk_management.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\NeCo_Git\NeCo\docs\sem_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373E1E4D-660E-45A5-8E2D-13757AB20998}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A1DE90-97B4-4863-AC53-0CF65840A088}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="6555" windowHeight="3668" xr2:uid="{CC889EFE-F9E2-4B7D-8E9D-18CCF3BDF79D}"/>
   </bookViews>
@@ -124,12 +124,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -162,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -172,6 +184,28 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -559,18 +593,18 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection sqref="A1:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="18.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.46484375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.9296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.86328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.9296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
@@ -596,7 +630,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>19</v>
       </c>
@@ -620,79 +654,79 @@
         <v>2.8000000000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="57" x14ac:dyDescent="0.45">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="8">
+        <v>5</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="8">
+        <f>PRODUCT(Tabelle4[[#This Row],[prob of occurence (in %)]:[damage/impact (1-10)]])</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C4" s="12">
         <v>0.3</v>
       </c>
-      <c r="D3">
+      <c r="D4" s="13">
         <v>7</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E4" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G3">
+      <c r="G4" s="13">
         <f>PRODUCT(Tabelle4[[#This Row],[prob of occurence (in %)]:[damage/impact (1-10)]])</f>
         <v>2.1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
-      <c r="E4" s="3" t="s">
+    <row r="5" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="D5" s="8">
         <v>10</v>
       </c>
-      <c r="F4" t="s">
+      <c r="E5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G4">
+      <c r="G5" s="8">
         <f>PRODUCT(Tabelle4[[#This Row],[prob of occurence (in %)]:[damage/impact (1-10)]])</f>
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5">
-        <f>PRODUCT(Tabelle4[[#This Row],[prob of occurence (in %)]:[damage/impact (1-10)]])</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -713,28 +747,28 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="D7">
+      <c r="C7" s="7">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D7" s="8">
         <v>8</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="8">
         <f>PRODUCT(Tabelle4[[#This Row],[prob of occurence (in %)]:[damage/impact (1-10)]])</f>
-        <v>0.16</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">

</xml_diff>